<commit_message>
Arvostelu valmis. Poisto ehkä valmis.
</commit_message>
<xml_diff>
--- a/VizPro_Final-Asiakas/Testiaineisto.xlsx
+++ b/VizPro_Final-Asiakas/Testiaineisto.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2323" uniqueCount="658">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2322" uniqueCount="657">
   <si>
     <t>Vuosi</t>
   </si>
@@ -2289,13 +2289,10 @@
 </t>
   </si>
   <si>
-    <t>3</t>
+    <t>6</t>
   </si>
   <si>
     <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
   </si>
 </sst>
 </file>
@@ -10747,10 +10744,10 @@
         <v>643</v>
       </c>
       <c r="Q160" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="R160" t="s">
-        <v>655</v>
+        <v>644</v>
       </c>
     </row>
     <row r="161">

</xml_diff>

<commit_message>
Lisäyssivun tarkistus, hakusivun toiminta korjattu
</commit_message>
<xml_diff>
--- a/VizPro_Final-Asiakas/Testiaineisto.xlsx
+++ b/VizPro_Final-Asiakas/Testiaineisto.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2320" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2466" uniqueCount="704">
   <si>
     <t>Vuosi</t>
   </si>
@@ -2286,6 +2286,213 @@
 null
 null
 null
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asd
+</t>
+  </si>
+  <si>
+    <t>testi</t>
+  </si>
+  <si>
+    <t>Testi</t>
+  </si>
+  <si>
+    <t>testimuoto</t>
+  </si>
+  <si>
+    <t>testikieli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. toiminta
+4. menetelmät
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Kartoitus (survey)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. haastattelu
+3. havainnointi
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Erityistyöntekijät: 
+5. potilaat/asiakkaat
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2 Toimintaprosessien arviointi
+2.4 Käytettävyys
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. koulutussektori
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null
+null
+</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>Fin 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Toimintaprosessien tiedon hallinnan organisointi ja ohjaus
+2. Tieto- ja viestintätekniikan käyttö
+4. Tietorakenteet- ja mallit
+null
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. toimijat
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. havainnointi
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Erityistyöntekijät: 
+</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2 Toimintaprosessien arviointi
+2.2 Käyttöönoton arviointi
+4.1.2 Rakenteiden kirjaaminen
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. kolmas sektori
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Toimintaprosessien tiedon hallinnan organisointi ja ohjaus
+2. Tieto- ja viestintätekniikan käyttö
+4. Tietorakenteet- ja mallit
+1. Toimintaprosessien tiedon hallinnan organisointi ja ohjaus
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sadasd
+</t>
+  </si>
+  <si>
+    <t>asdasd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. Toimintatutkimus
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6. kansalaiset
+</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.2 Toimintaprosessien arviointi
+2.3 Sähköinen asiointi
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. erikoissairaanhoito
+</t>
+  </si>
+  <si>
+    <t>testitesti</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Toimintaprosessien tiedon hallinnan organisointi ja ohjaus
+2. Tieto- ja viestintätekniikan käyttö
+1. Toimintaprosessien tiedon hallinnan organisointi ja ohjaus
+2. Tieto- ja viestintätekniikan käyttö
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Toimintaprosessien tiedon hallinnan organisointi ja ohjaus
+null
+null
+null
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. tieto
+2. toimijat
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7. Arviointitutkimus
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. haastattelu
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9. johtajat
+</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.1 Toimintaprosessien mallinnus
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. yksityissektori
+</t>
+  </si>
+  <si>
+    <t>asda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. Lääkärit
+</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.4 Informaatioetiikka
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. sosiaalihuolto
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null
+null
+null
+null
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Asiakirjat: 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sad
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. menetelmät
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. Delfoi
 </t>
   </si>
 </sst>
@@ -2363,7 +2570,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2394,6 +2601,222 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true"/>
     </xf>
@@ -2722,7 +3145,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R161"/>
+  <dimension ref="A1:R170"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A155" workbookViewId="0">
       <selection activeCell="Q14" sqref="Q14"/>
@@ -10795,6 +11218,496 @@
         <v>644</v>
       </c>
       <c r="R161" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="B162" s="34" t="s">
+        <v>655</v>
+      </c>
+      <c r="C162" t="s">
+        <v>656</v>
+      </c>
+      <c r="D162" t="s">
+        <v>657</v>
+      </c>
+      <c r="E162" t="s">
+        <v>658</v>
+      </c>
+      <c r="F162" t="s">
+        <v>635</v>
+      </c>
+      <c r="G162" t="s">
+        <v>659</v>
+      </c>
+      <c r="H162" t="s">
+        <v>23</v>
+      </c>
+      <c r="I162" s="35" t="s">
+        <v>636</v>
+      </c>
+      <c r="J162" s="36" t="s">
+        <v>660</v>
+      </c>
+      <c r="K162" s="37" t="s">
+        <v>661</v>
+      </c>
+      <c r="L162" s="38" t="s">
+        <v>662</v>
+      </c>
+      <c r="M162" s="39" t="s">
+        <v>663</v>
+      </c>
+      <c r="N162" t="s">
+        <v>641</v>
+      </c>
+      <c r="O162" s="40" t="s">
+        <v>664</v>
+      </c>
+      <c r="P162" s="41" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q162" t="s">
+        <v>644</v>
+      </c>
+      <c r="R162" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>2004.0</v>
+      </c>
+      <c r="B163" s="42" t="s">
+        <v>666</v>
+      </c>
+      <c r="C163" t="s">
+        <v>667</v>
+      </c>
+      <c r="D163" t="s">
+        <v>20</v>
+      </c>
+      <c r="E163" t="s">
+        <v>21</v>
+      </c>
+      <c r="F163" t="s">
+        <v>668</v>
+      </c>
+      <c r="G163" t="s">
+        <v>22</v>
+      </c>
+      <c r="H163" t="s">
+        <v>52</v>
+      </c>
+      <c r="I163" s="43" t="s">
+        <v>669</v>
+      </c>
+      <c r="J163" s="44" t="s">
+        <v>670</v>
+      </c>
+      <c r="K163" s="45" t="s">
+        <v>661</v>
+      </c>
+      <c r="L163" s="46" t="s">
+        <v>671</v>
+      </c>
+      <c r="M163" s="47" t="s">
+        <v>672</v>
+      </c>
+      <c r="N163" t="s">
+        <v>673</v>
+      </c>
+      <c r="O163" s="48" t="s">
+        <v>674</v>
+      </c>
+      <c r="P163" s="49" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q163" t="s">
+        <v>644</v>
+      </c>
+      <c r="R163" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="n">
+        <v>2004.0</v>
+      </c>
+      <c r="B164" s="50" t="s">
+        <v>666</v>
+      </c>
+      <c r="C164" t="s">
+        <v>667</v>
+      </c>
+      <c r="D164" t="s">
+        <v>20</v>
+      </c>
+      <c r="E164" t="s">
+        <v>21</v>
+      </c>
+      <c r="F164" t="s">
+        <v>668</v>
+      </c>
+      <c r="G164" t="s">
+        <v>22</v>
+      </c>
+      <c r="H164" t="s">
+        <v>52</v>
+      </c>
+      <c r="I164" s="51" t="s">
+        <v>676</v>
+      </c>
+      <c r="J164" s="52" t="s">
+        <v>670</v>
+      </c>
+      <c r="K164" s="53" t="s">
+        <v>661</v>
+      </c>
+      <c r="L164" s="54" t="s">
+        <v>671</v>
+      </c>
+      <c r="M164" s="55" t="s">
+        <v>672</v>
+      </c>
+      <c r="N164" t="s">
+        <v>673</v>
+      </c>
+      <c r="O164" s="56" t="s">
+        <v>674</v>
+      </c>
+      <c r="P164" s="57" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q164" t="s">
+        <v>644</v>
+      </c>
+      <c r="R164" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="B165" s="58" t="s">
+        <v>677</v>
+      </c>
+      <c r="C165" t="s">
+        <v>678</v>
+      </c>
+      <c r="D165" t="s">
+        <v>20</v>
+      </c>
+      <c r="E165" t="s">
+        <v>21</v>
+      </c>
+      <c r="F165" t="s">
+        <v>635</v>
+      </c>
+      <c r="G165" t="s">
+        <v>22</v>
+      </c>
+      <c r="H165" t="s">
+        <v>23</v>
+      </c>
+      <c r="I165" s="59" t="s">
+        <v>636</v>
+      </c>
+      <c r="J165" s="60" t="s">
+        <v>670</v>
+      </c>
+      <c r="K165" s="61" t="s">
+        <v>679</v>
+      </c>
+      <c r="L165" s="62" t="s">
+        <v>671</v>
+      </c>
+      <c r="M165" s="63" t="s">
+        <v>680</v>
+      </c>
+      <c r="N165" t="s">
+        <v>681</v>
+      </c>
+      <c r="O165" s="64" t="s">
+        <v>682</v>
+      </c>
+      <c r="P165" s="65" t="s">
+        <v>683</v>
+      </c>
+      <c r="Q165" t="s">
+        <v>644</v>
+      </c>
+      <c r="R165" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="B166" s="66" t="s">
+        <v>677</v>
+      </c>
+      <c r="C166" t="s">
+        <v>684</v>
+      </c>
+      <c r="D166" t="s">
+        <v>20</v>
+      </c>
+      <c r="E166" t="s">
+        <v>21</v>
+      </c>
+      <c r="F166" t="s">
+        <v>635</v>
+      </c>
+      <c r="G166" t="s">
+        <v>22</v>
+      </c>
+      <c r="H166" t="s">
+        <v>23</v>
+      </c>
+      <c r="I166" s="67" t="s">
+        <v>685</v>
+      </c>
+      <c r="J166" s="68" t="s">
+        <v>670</v>
+      </c>
+      <c r="K166" s="69" t="s">
+        <v>679</v>
+      </c>
+      <c r="L166" s="70" t="s">
+        <v>671</v>
+      </c>
+      <c r="M166" s="71" t="s">
+        <v>680</v>
+      </c>
+      <c r="N166" t="s">
+        <v>681</v>
+      </c>
+      <c r="O166" s="72" t="s">
+        <v>682</v>
+      </c>
+      <c r="P166" s="73" t="s">
+        <v>683</v>
+      </c>
+      <c r="Q166" t="s">
+        <v>644</v>
+      </c>
+      <c r="R166" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="B167" s="74" t="s">
+        <v>666</v>
+      </c>
+      <c r="C167" t="s">
+        <v>678</v>
+      </c>
+      <c r="D167" t="s">
+        <v>20</v>
+      </c>
+      <c r="E167" t="s">
+        <v>21</v>
+      </c>
+      <c r="F167" t="s">
+        <v>635</v>
+      </c>
+      <c r="G167" t="s">
+        <v>22</v>
+      </c>
+      <c r="H167" t="s">
+        <v>52</v>
+      </c>
+      <c r="I167" s="75" t="s">
+        <v>686</v>
+      </c>
+      <c r="J167" s="76" t="s">
+        <v>687</v>
+      </c>
+      <c r="K167" s="77" t="s">
+        <v>688</v>
+      </c>
+      <c r="L167" s="78" t="s">
+        <v>689</v>
+      </c>
+      <c r="M167" s="79" t="s">
+        <v>690</v>
+      </c>
+      <c r="N167" t="s">
+        <v>691</v>
+      </c>
+      <c r="O167" s="80" t="s">
+        <v>692</v>
+      </c>
+      <c r="P167" s="81" t="s">
+        <v>693</v>
+      </c>
+      <c r="Q167" t="s">
+        <v>644</v>
+      </c>
+      <c r="R167" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="n">
+        <v>2004.0</v>
+      </c>
+      <c r="B168" s="82" t="s">
+        <v>655</v>
+      </c>
+      <c r="C168" t="s">
+        <v>694</v>
+      </c>
+      <c r="D168" t="s">
+        <v>20</v>
+      </c>
+      <c r="E168" t="s">
+        <v>21</v>
+      </c>
+      <c r="F168" t="s">
+        <v>668</v>
+      </c>
+      <c r="G168" t="s">
+        <v>22</v>
+      </c>
+      <c r="H168" t="s">
+        <v>23</v>
+      </c>
+      <c r="I168" s="83" t="s">
+        <v>686</v>
+      </c>
+      <c r="J168" s="84" t="s">
+        <v>670</v>
+      </c>
+      <c r="K168" s="85" t="s">
+        <v>679</v>
+      </c>
+      <c r="L168" s="86" t="s">
+        <v>671</v>
+      </c>
+      <c r="M168" s="87" t="s">
+        <v>695</v>
+      </c>
+      <c r="N168" t="s">
+        <v>696</v>
+      </c>
+      <c r="O168" s="88" t="s">
+        <v>697</v>
+      </c>
+      <c r="P168" s="89" t="s">
+        <v>698</v>
+      </c>
+      <c r="Q168" t="s">
+        <v>644</v>
+      </c>
+      <c r="R168" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="n">
+        <v>2005.0</v>
+      </c>
+      <c r="B169" s="90" t="s">
+        <v>666</v>
+      </c>
+      <c r="C169" t="s">
+        <v>667</v>
+      </c>
+      <c r="D169"/>
+      <c r="E169"/>
+      <c r="F169" t="s">
+        <v>635</v>
+      </c>
+      <c r="G169"/>
+      <c r="H169" t="s">
+        <v>52</v>
+      </c>
+      <c r="I169" s="91" t="s">
+        <v>699</v>
+      </c>
+      <c r="J169" s="92" t="s">
+        <v>670</v>
+      </c>
+      <c r="K169" s="93" t="s">
+        <v>688</v>
+      </c>
+      <c r="L169" s="94" t="s">
+        <v>700</v>
+      </c>
+      <c r="M169" s="95" t="s">
+        <v>680</v>
+      </c>
+      <c r="N169" t="s">
+        <v>641</v>
+      </c>
+      <c r="O169" s="96" t="s">
+        <v>641</v>
+      </c>
+      <c r="P169" s="97" t="s">
+        <v>675</v>
+      </c>
+      <c r="Q169" t="s">
+        <v>644</v>
+      </c>
+      <c r="R169" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="n">
+        <v>2004.0</v>
+      </c>
+      <c r="B170" s="98" t="s">
+        <v>701</v>
+      </c>
+      <c r="C170" t="s">
+        <v>667</v>
+      </c>
+      <c r="D170"/>
+      <c r="E170"/>
+      <c r="F170"/>
+      <c r="G170"/>
+      <c r="H170" t="s">
+        <v>23</v>
+      </c>
+      <c r="I170" s="99" t="s">
+        <v>699</v>
+      </c>
+      <c r="J170" s="100" t="s">
+        <v>702</v>
+      </c>
+      <c r="K170" s="101" t="s">
+        <v>703</v>
+      </c>
+      <c r="L170" s="102" t="s">
+        <v>671</v>
+      </c>
+      <c r="M170" s="103" t="s">
+        <v>680</v>
+      </c>
+      <c r="N170" t="s">
+        <v>641</v>
+      </c>
+      <c r="O170" s="104" t="s">
+        <v>641</v>
+      </c>
+      <c r="P170" s="105" t="s">
+        <v>665</v>
+      </c>
+      <c r="Q170" t="s">
+        <v>644</v>
+      </c>
+      <c r="R170" t="s">
         <v>644</v>
       </c>
     </row>

</xml_diff>